<commit_message>
Finalize ERD and Data Dictionary
Updated the ERD and Data Dictionary.
</commit_message>
<xml_diff>
--- a/Phase 2/Data Dictionary.xlsx
+++ b/Phase 2/Data Dictionary.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B87FDC-86A6-408C-8990-5B6A422FD731}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4E5C43-5755-4E8E-BB77-D6E7A14D5E31}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="11388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="972" windowWidth="17280" windowHeight="11388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="104">
   <si>
     <t>Table</t>
   </si>
@@ -215,20 +215,146 @@
   </si>
   <si>
     <t>Driver Type</t>
+  </si>
+  <si>
+    <t>1594 Balcerzak Dr.</t>
+  </si>
+  <si>
+    <t>Number of MVR Order within the year</t>
+  </si>
+  <si>
+    <t>Viol</t>
+  </si>
+  <si>
+    <t>Hit/Run</t>
+  </si>
+  <si>
+    <t>as1548er</t>
+  </si>
+  <si>
+    <t>Qwer1234</t>
+  </si>
+  <si>
+    <t>Auto dealer</t>
+  </si>
+  <si>
+    <t>1234 Madison Ave</t>
+  </si>
+  <si>
+    <t>(507)159-4897</t>
+  </si>
+  <si>
+    <t>John.Doe@Auto.com</t>
+  </si>
+  <si>
+    <t>Bob.Fisher@Auto.com</t>
+  </si>
+  <si>
+    <t>Driver Type ID</t>
+  </si>
+  <si>
+    <t>Truck Driver</t>
+  </si>
+  <si>
+    <t>Unique ID for Driver Type</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Unique ID for MVR</t>
+  </si>
+  <si>
+    <t>Status of MVR</t>
+  </si>
+  <si>
+    <t>Sent</t>
+  </si>
+  <si>
+    <t>Date of MVR request</t>
+  </si>
+  <si>
+    <t>Date of MVR report</t>
+  </si>
+  <si>
+    <t>Unique Violation Code</t>
+  </si>
+  <si>
+    <t>Date of Violation</t>
+  </si>
+  <si>
+    <t>Location of Violation</t>
+  </si>
+  <si>
+    <t>Description of Violation</t>
+  </si>
+  <si>
+    <t>Type of Violation</t>
+  </si>
+  <si>
+    <t>Amount of violation</t>
+  </si>
+  <si>
+    <t>Suspension date</t>
+  </si>
+  <si>
+    <t>Conviction date</t>
+  </si>
+  <si>
+    <t>Unique Underwriter ID</t>
+  </si>
+  <si>
+    <t>Unique Company ID</t>
+  </si>
+  <si>
+    <t>Name of Company</t>
+  </si>
+  <si>
+    <t>Underwriter username</t>
+  </si>
+  <si>
+    <t>Underwriter password</t>
+  </si>
+  <si>
+    <t>Company Address</t>
+  </si>
+  <si>
+    <t>Company City</t>
+  </si>
+  <si>
+    <t>Company State</t>
+  </si>
+  <si>
+    <t>Company Zip</t>
+  </si>
+  <si>
+    <t>Company phone</t>
+  </si>
+  <si>
+    <t>Company Rep Email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m\-yyyy"/>
+  <numFmts count="3">
     <numFmt numFmtId="165" formatCode="m\-d\-yyyy"/>
+    <numFmt numFmtId="166" formatCode="00000"/>
+    <numFmt numFmtId="168" formatCode="m/d/yy;@"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -257,10 +383,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -269,9 +396,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -283,8 +407,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -563,19 +700,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.33203125" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.44140625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.21875" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -588,7 +725,7 @@
       <c r="C1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -695,7 +832,7 @@
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>43570</v>
       </c>
       <c r="D7" s="2">
@@ -803,206 +940,328 @@
       <c r="B13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="E13" s="1"/>
+      <c r="C13" s="8">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="B14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="4">
+        <v>15948</v>
+      </c>
+      <c r="D14" s="2">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>18</v>
+      <c r="C15" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="D15" s="2">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="C16" s="4"/>
       <c r="D16" s="2">
         <v>25</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1">
+        <v>159159159</v>
+      </c>
+      <c r="D17" s="2">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="2">
+        <v>25</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="2">
+      <c r="C19" s="5">
+        <v>43572</v>
+      </c>
+      <c r="D19" s="2">
         <v>8</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B18" s="1" t="s">
+      <c r="F19" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="2">
+      <c r="C20" s="5">
+        <v>43480</v>
+      </c>
+      <c r="D20" s="2">
         <v>8</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B19" s="1" t="s">
+      <c r="F20" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D21" s="2">
         <v>50</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="E21" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="C22" s="7">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
+        <v>5</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B21" s="1" t="s">
+      <c r="F22" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="2">
+      <c r="C23" s="5">
+        <v>43515</v>
+      </c>
+      <c r="D23" s="2">
         <v>8</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
+      <c r="F23" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B23" s="1" t="s">
+      <c r="C24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="2">
+      <c r="C25" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" s="2">
         <v>50</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="1" t="s">
+      <c r="E25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
+      <c r="C26" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D26" s="2">
+        <v>10</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="2">
+      <c r="C27" s="1">
+        <v>5</v>
+      </c>
+      <c r="D27" s="2">
         <v>2</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="1" t="s">
+      <c r="F27" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B27" s="1" t="s">
+      <c r="C28" s="9">
+        <v>42232</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+      <c r="C29" s="9">
+        <v>42257</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="2">
+      <c r="C30" s="1">
+        <v>456123789</v>
+      </c>
+      <c r="D30" s="2">
         <v>9</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B29" s="1" t="s">
+      <c r="F30" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="2">
+      <c r="C31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="2">
         <v>15</v>
       </c>
-      <c r="E29" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B30" s="1" t="s">
+      <c r="E31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="2">
-        <v>15</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="2">
-        <v>9</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B32" s="1" t="s">
-        <v>46</v>
+      <c r="C32" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="D32" s="2">
         <v>15</v>
@@ -1010,21 +1269,36 @@
       <c r="E32" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F32" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>44</v>
+      </c>
       <c r="B33" s="1" t="s">
-        <v>12</v>
+        <v>45</v>
+      </c>
+      <c r="C33" s="1">
+        <v>159487564</v>
       </c>
       <c r="D33" s="2">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
-        <v>13</v>
+        <v>46</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="D34" s="2">
         <v>15</v>
@@ -1032,71 +1306,142 @@
       <c r="E34" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F34" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="2">
+        <v>50</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D36" s="2">
+        <v>15</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B37" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="2">
+      <c r="C37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" s="2">
         <v>2</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B36" s="1" t="s">
+      <c r="E37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="2">
+      <c r="C38" s="1">
+        <v>56001</v>
+      </c>
+      <c r="D38" s="2">
         <v>5</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B37" s="1" t="s">
+      <c r="F38" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B39" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="2">
+      <c r="C39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B38" s="1" t="s">
+      <c r="F39" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B40" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D38" s="2">
+      <c r="C40" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="2">
         <v>25</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B39" s="1" t="s">
+      <c r="E40" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B41" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="2">
+      <c r="C41" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="2">
         <v>25</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B41" s="1"/>
+      <c r="E41" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B42" s="1"/>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B43" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C40" r:id="rId1" xr:uid="{114DC1D7-4E7D-434F-8675-0684CDCA83BC}"/>
+    <hyperlink ref="C41" r:id="rId2" xr:uid="{160FEF2C-4E1B-471A-A608-DBF57A0B053D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>